<commit_message>
arreglo en todos los archivos para la pestaña de cada interface
</commit_message>
<xml_diff>
--- a/matriculas.xlsx
+++ b/matriculas.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,9 +441,8 @@
   <cols>
     <col width="12" customWidth="1" min="1" max="1"/>
     <col width="34" customWidth="1" min="2" max="2"/>
-    <col width="6" customWidth="1" min="3" max="3"/>
-    <col width="11" customWidth="1" min="4" max="4"/>
-    <col width="7" customWidth="1" min="5" max="5"/>
+    <col width="17" customWidth="1" min="3" max="3"/>
+    <col width="18" customWidth="1" min="4" max="4"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -459,17 +458,12 @@
       </c>
       <c r="C1" s="2" t="inlineStr">
         <is>
-          <t>Edad</t>
+          <t>Fecha Matrícula</t>
         </is>
       </c>
       <c r="D1" s="2" t="inlineStr">
         <is>
-          <t>Modalidad</t>
-        </is>
-      </c>
-      <c r="E1" s="2" t="inlineStr">
-        <is>
-          <t>Peso</t>
+          <t>Correo</t>
         </is>
       </c>
     </row>
@@ -486,17 +480,34 @@
       </c>
       <c r="C2" s="3" t="inlineStr">
         <is>
-          <t>25</t>
+          <t>2025-01-04</t>
         </is>
       </c>
       <c r="D2" s="3" t="inlineStr">
         <is>
-          <t>Boxeo</t>
-        </is>
-      </c>
-      <c r="E2" s="3" t="inlineStr">
-        <is>
-          <t>54 kg</t>
+          <t>paola@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="inlineStr">
+        <is>
+          <t>1716776412</t>
+        </is>
+      </c>
+      <c r="B3" s="3" t="inlineStr">
+        <is>
+          <t>hfgfghfgh fghfghfgh</t>
+        </is>
+      </c>
+      <c r="C3" s="3" t="inlineStr">
+        <is>
+          <t>2025-02-23</t>
+        </is>
+      </c>
+      <c r="D3" s="3" t="inlineStr">
+        <is>
+          <t>darwi@ngmail.com</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
validacion de modulos, y cambios en la pagina web
</commit_message>
<xml_diff>
--- a/matriculas.xlsx
+++ b/matriculas.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,8 +441,9 @@
   <cols>
     <col width="12" customWidth="1" min="1" max="1"/>
     <col width="34" customWidth="1" min="2" max="2"/>
-    <col width="17" customWidth="1" min="3" max="3"/>
-    <col width="18" customWidth="1" min="4" max="4"/>
+    <col width="6" customWidth="1" min="3" max="3"/>
+    <col width="11" customWidth="1" min="4" max="4"/>
+    <col width="7" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -458,12 +459,17 @@
       </c>
       <c r="C1" s="2" t="inlineStr">
         <is>
-          <t>Fecha Matrícula</t>
+          <t>Edad</t>
         </is>
       </c>
       <c r="D1" s="2" t="inlineStr">
         <is>
-          <t>Correo</t>
+          <t>Modalidad</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>Peso</t>
         </is>
       </c>
     </row>
@@ -480,34 +486,44 @@
       </c>
       <c r="C2" s="3" t="inlineStr">
         <is>
-          <t>2025-01-04</t>
+          <t>25</t>
         </is>
       </c>
       <c r="D2" s="3" t="inlineStr">
         <is>
-          <t>paola@gmail.com</t>
+          <t>Boxeo</t>
+        </is>
+      </c>
+      <c r="E2" s="3" t="inlineStr">
+        <is>
+          <t>54 kg</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>1716776412</t>
+          <t>1750321901</t>
         </is>
       </c>
       <c r="B3" s="3" t="inlineStr">
         <is>
-          <t>hfgfghfgh fghfghfgh</t>
+          <t>AngeloO Lopez</t>
         </is>
       </c>
       <c r="C3" s="3" t="inlineStr">
         <is>
-          <t>2025-02-23</t>
+          <t>21</t>
         </is>
       </c>
       <c r="D3" s="3" t="inlineStr">
         <is>
-          <t>darwi@ngmail.com</t>
+          <t>Boxeo</t>
+        </is>
+      </c>
+      <c r="E3" s="3" t="inlineStr">
+        <is>
+          <t>58 kg</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
modificacion de algunos modulos
</commit_message>
<xml_diff>
--- a/matriculas.xlsx
+++ b/matriculas.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -442,7 +442,7 @@
     <col width="12" customWidth="1" min="1" max="1"/>
     <col width="34" customWidth="1" min="2" max="2"/>
     <col width="6" customWidth="1" min="3" max="3"/>
-    <col width="11" customWidth="1" min="4" max="4"/>
+    <col width="13" customWidth="1" min="4" max="4"/>
     <col width="7" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>
@@ -508,7 +508,7 @@
       </c>
       <c r="B3" s="3" t="inlineStr">
         <is>
-          <t>AngeloO Lopez</t>
+          <t>Angelo Lopez</t>
         </is>
       </c>
       <c r="C3" s="3" t="inlineStr">
@@ -524,6 +524,60 @@
       <c r="E3" s="3" t="inlineStr">
         <is>
           <t>58 kg</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="inlineStr">
+        <is>
+          <t>1716776412</t>
+        </is>
+      </c>
+      <c r="B4" s="3" t="inlineStr">
+        <is>
+          <t>Darwin Vinicio Cruz Guanga</t>
+        </is>
+      </c>
+      <c r="C4" s="3" t="inlineStr">
+        <is>
+          <t>44</t>
+        </is>
+      </c>
+      <c r="D4" s="3" t="inlineStr">
+        <is>
+          <t>Boxeo</t>
+        </is>
+      </c>
+      <c r="E4" s="3" t="inlineStr">
+        <is>
+          <t>48 kg</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="inlineStr">
+        <is>
+          <t>1751566785</t>
+        </is>
+      </c>
+      <c r="B5" s="3" t="inlineStr">
+        <is>
+          <t>Roberto Carlos</t>
+        </is>
+      </c>
+      <c r="C5" s="3" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="D5" s="3" t="inlineStr">
+        <is>
+          <t>Kick Boxing</t>
+        </is>
+      </c>
+      <c r="E5" s="3" t="inlineStr">
+        <is>
+          <t>69 kg</t>
         </is>
       </c>
     </row>

</xml_diff>